<commit_message>
update congregations.py et 40CM_coll_iiif.py
</commit_message>
<xml_diff>
--- a/iiif/40CM_coll_iiif.xlsx
+++ b/iiif/40CM_coll_iiif.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rebecca\Documents\GitHub\SHERLOCK\iiif\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF4743F-0886-4A02-A42D-343961B9D6DB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889F1F43-71FB-442E-95CF-BA99ABB6F436}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{ABDC5E25-0FA4-41BE-9150-9BDB7AE3A285}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ABDC5E25-0FA4-41BE-9150-9BDB7AE3A285}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,26 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>collection</t>
   </si>
   <si>
-    <t>responsable</t>
-  </si>
-  <si>
-    <t>type de collection</t>
-  </si>
-  <si>
-    <t>licence</t>
-  </si>
-  <si>
-    <t>description de la collection</t>
-  </si>
-  <si>
-    <t>Livre</t>
-  </si>
-  <si>
     <t>n° de page**</t>
   </si>
   <si>
@@ -67,68 +51,23 @@
     <t>nom de l'image*</t>
   </si>
   <si>
-    <t>Les 40 chanteurs montagnards</t>
-  </si>
-  <si>
-    <t>Nicolas Dufétel</t>
-  </si>
-  <si>
-    <t>titre du livre**</t>
-  </si>
-  <si>
-    <t>date de publication**</t>
-  </si>
-  <si>
-    <t>lieu de publication**</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>40CM</t>
   </si>
   <si>
-    <t>Publication numérisée.</t>
-  </si>
-  <si>
-    <t>https://creativecommons.org/publicdomain/zero/1.0/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">créateur-ice de l'œuvre (si différent-e de l'auteur-e) </t>
-  </si>
-  <si>
-    <t>auteur-e**</t>
-  </si>
-  <si>
-    <t>date de conception de l'œuvre (si différente de la date de publication)**</t>
-  </si>
-  <si>
-    <t>auteur inconnu</t>
-  </si>
-  <si>
-    <t>date inconnue</t>
-  </si>
-  <si>
-    <t>lieu inconnu</t>
-  </si>
-  <si>
-    <t>créateur inconnu</t>
-  </si>
-  <si>
-    <t>0000-0000</t>
-  </si>
-  <si>
-    <t>type d'image</t>
-  </si>
-  <si>
-    <t>page</t>
+    <t>type d'image*</t>
+  </si>
+  <si>
+    <t>contient une image**</t>
+  </si>
+  <si>
+    <t>oui</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,11 +97,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -190,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -204,10 +138,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -215,15 +149,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -541,14 +466,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F379C2-2FF4-4130-9DA9-93CB115680B5}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19.05" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19.05" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="30.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" style="6" customWidth="1"/>
     <col min="4" max="4" width="30.44140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="25.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="31.109375" style="2" customWidth="1"/>
@@ -560,62 +485,68 @@
     <col min="14" max="16384" width="11.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1" ht="19.05" customHeight="1">
+    <row r="1" spans="1:5" s="3" customFormat="1" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
     </row>
-    <row r="2" spans="1:5" ht="19.05" customHeight="1">
+    <row r="2" spans="1:5" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
     </row>
-    <row r="4" spans="1:5" s="4" customFormat="1" ht="18.600000000000001" customHeight="1">
+    <row r="4" spans="1:5" s="4" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="9" t="s">
         <v>6</v>
       </c>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19.05" customHeight="1">
+    <row r="5" spans="1:5" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="10">
+        <v>5</v>
+      </c>
+      <c r="C5" s="6">
         <v>1</v>
       </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="19.05" customHeight="1">
+    <row r="6" spans="1:5" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="10">
+        <v>5</v>
+      </c>
+      <c r="C6" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="19.05" customHeight="1">
+    <row r="7" spans="1:5" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="10">
+        <v>5</v>
+      </c>
+      <c r="C7" s="6">
         <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -627,125 +558,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDBF2167-B86A-4BF9-A1E6-BD283645A530}">
-  <dimension ref="A1:L5"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.77734375" defaultRowHeight="18" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="31.44140625" customWidth="1"/>
-    <col min="6" max="6" width="25.33203125" customWidth="1"/>
-    <col min="7" max="7" width="24.21875" customWidth="1"/>
-    <col min="8" max="8" width="38.109375" customWidth="1"/>
-    <col min="10" max="10" width="27" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" ht="18.600000000000001" customHeight="1">
-      <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:12" ht="18" customHeight="1">
-      <c r="A2" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:12" ht="38.4" customHeight="1"/>
-    <row r="4" spans="1:12" ht="61.2" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="44.4" customHeight="1">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>